<commit_message>
20170808T2115 - EO Setup and harmonisation of introduction to criteria-2
</commit_message>
<xml_diff>
--- a/docs/src/main/asciidoc/dist/cl/xlsx/ESPDRequest-CriteriaTaxonomy-REGULATED-V02.00.00.xlsx
+++ b/docs/src/main/asciidoc/dist/cl/xlsx/ESPDRequest-CriteriaTaxonomy-REGULATED-V02.00.00.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="20730" windowHeight="8400" firstSheet="9" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="20730" windowHeight="8400" firstSheet="7" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="EG-Convictions" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14455" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14455" uniqueCount="400">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1271,6 +1271,12 @@
   <si>
     <t xml:space="preserve">  </t>
   </si>
+  <si>
+    <t>696a75b2-6107-428f-8b74-82affb67e184</t>
+  </si>
+  <si>
+    <t>CRITERION.EXCLUSION.CONFLICT_OF_INTEREST.MISINTERPRETATION</t>
+  </si>
 </sst>
 </file>
 
@@ -2002,7 +2008,7 @@
     <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="130">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2345,6 +2351,12 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -13038,7 +13050,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+    <sheetView topLeftCell="A24" workbookViewId="0">
       <selection activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
@@ -16876,7 +16888,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:N8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -16884,7 +16898,9 @@
     <col min="2" max="2" width="11.42578125" style="35" customWidth="1"/>
     <col min="3" max="3" width="21.85546875" style="35" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" style="35" customWidth="1"/>
-    <col min="5" max="16384" width="11.42578125" style="35"/>
+    <col min="5" max="9" width="11.42578125" style="35"/>
+    <col min="10" max="11" width="0" style="35" hidden="1" customWidth="1"/>
+    <col min="12" max="16384" width="11.42578125" style="35"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
@@ -17085,25 +17101,25 @@
       <c r="B5" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="I5" s="8" t="s">
+      <c r="D5" s="64" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="64" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="64" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" s="64" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5" s="64" t="s">
+        <v>0</v>
+      </c>
+      <c r="I5" s="65" t="s">
         <v>0</v>
       </c>
       <c r="J5" s="8" t="s">
@@ -17132,25 +17148,25 @@
       <c r="B6" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="8" t="s">
+      <c r="C6" s="66" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="I6" s="8" t="s">
+      <c r="E6" s="67" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="67" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" s="67" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" s="67" t="s">
+        <v>0</v>
+      </c>
+      <c r="I6" s="68" t="s">
         <v>226</v>
       </c>
       <c r="J6" s="8" t="s">
@@ -17179,25 +17195,25 @@
       <c r="B7" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="I7" s="5" t="s">
+      <c r="D7" s="128" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="128" t="s">
+        <v>0</v>
+      </c>
+      <c r="F7" s="128" t="s">
+        <v>0</v>
+      </c>
+      <c r="G7" s="128" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7" s="128" t="s">
+        <v>0</v>
+      </c>
+      <c r="I7" s="129" t="s">
         <v>0</v>
       </c>
       <c r="J7" s="5" t="s">
@@ -50371,7 +50387,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -50517,10 +50535,10 @@
         <v>0</v>
       </c>
       <c r="M3" s="92" t="s">
-        <v>166</v>
+        <v>398</v>
       </c>
       <c r="N3" s="82" t="s">
-        <v>167</v>
+        <v>399</v>
       </c>
       <c r="O3" s="31" t="s">
         <v>171</v>

</xml_diff>

<commit_message>
20170808T2253 - Regulated and Self-contained Financial Ratios added.
</commit_message>
<xml_diff>
--- a/docs/src/main/asciidoc/dist/cl/xlsx/ESPDRequest-CriteriaTaxonomy-REGULATED-V02.00.00.xlsx
+++ b/docs/src/main/asciidoc/dist/cl/xlsx/ESPDRequest-CriteriaTaxonomy-REGULATED-V02.00.00.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="20730" windowHeight="8400" firstSheet="7" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="20730" windowHeight="8400" firstSheet="11" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="EG-Convictions" sheetId="1" r:id="rId1"/>
@@ -17292,16 +17292,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" style="29" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" style="28" customWidth="1"/>
     <col min="3" max="3" width="18.140625" style="28" customWidth="1"/>
-    <col min="4" max="5" width="25.42578125" style="28" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" style="28" customWidth="1"/>
-    <col min="7" max="16384" width="11.42578125" style="28"/>
+    <col min="4" max="4" width="25.42578125" style="28" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" style="28" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="1.85546875" style="28" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="28" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" style="28" customWidth="1"/>
+    <col min="10" max="11" width="0" style="28" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="17.140625" style="28" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="11.42578125" style="28"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -17499,25 +17506,25 @@
       <c r="B5" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="I5" s="8" t="s">
+      <c r="D5" s="64" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="64" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="64" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" s="64" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5" s="64" t="s">
+        <v>0</v>
+      </c>
+      <c r="I5" s="65" t="s">
         <v>0</v>
       </c>
       <c r="J5" s="8" t="s">
@@ -17546,25 +17553,25 @@
       <c r="B6" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="8" t="s">
+      <c r="C6" s="66" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="I6" s="8" t="s">
+      <c r="E6" s="64" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="64" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" s="64" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" s="64" t="s">
+        <v>0</v>
+      </c>
+      <c r="I6" s="65" t="s">
         <v>0</v>
       </c>
       <c r="J6" s="8" t="s">
@@ -17593,25 +17600,25 @@
       <c r="B7" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E7" s="8" t="s">
+      <c r="C7" s="66" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="66" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="I7" s="8" t="s">
+      <c r="F7" s="67" t="s">
+        <v>0</v>
+      </c>
+      <c r="G7" s="67" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7" s="67" t="s">
+        <v>0</v>
+      </c>
+      <c r="I7" s="68" t="s">
         <v>384</v>
       </c>
       <c r="J7" s="8" t="s">
@@ -17640,25 +17647,25 @@
       <c r="B8" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="8" t="s">
+      <c r="C8" s="66" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="E8" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="I8" s="8" t="s">
+      <c r="E8" s="70" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" s="70" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" s="70" t="s">
+        <v>0</v>
+      </c>
+      <c r="H8" s="70" t="s">
+        <v>0</v>
+      </c>
+      <c r="I8" s="71" t="s">
         <v>0</v>
       </c>
       <c r="J8" s="8" t="s">
@@ -17687,25 +17694,25 @@
       <c r="B9" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="I9" s="8" t="s">
+      <c r="D9" s="70" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" s="70" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" s="70" t="s">
+        <v>0</v>
+      </c>
+      <c r="G9" s="70" t="s">
+        <v>0</v>
+      </c>
+      <c r="H9" s="70" t="s">
+        <v>0</v>
+      </c>
+      <c r="I9" s="71" t="s">
         <v>0</v>
       </c>
       <c r="J9" s="8" t="s">
@@ -50387,7 +50394,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
20170831T2316 - EO XSDs and Data Structures (1)
</commit_message>
<xml_diff>
--- a/docs/src/main/asciidoc/dist/cl/xlsx/ESPDRequest-CriteriaTaxonomy-REGULATED-V02.00.00.xlsx
+++ b/docs/src/main/asciidoc/dist/cl/xlsx/ESPDRequest-CriteriaTaxonomy-REGULATED-V02.00.00.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="20730" windowHeight="8400" firstSheet="17" activeTab="21"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="20730" windowHeight="8400" firstSheet="17" activeTab="23"/>
   </bookViews>
   <sheets>
     <sheet name="EG-Convictions" sheetId="1" r:id="rId1"/>
@@ -30,13 +30,14 @@
     <sheet name="SC-Subcontracting_proportion" sheetId="20" r:id="rId21"/>
     <sheet name="SC-Samples_certificates" sheetId="21" r:id="rId22"/>
     <sheet name="SC-Quality_assurance" sheetId="22" r:id="rId23"/>
+    <sheet name="OTHER-PQS" sheetId="24" r:id="rId24"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12087" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12183" uniqueCount="391">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1232,6 +1233,24 @@
   <si>
     <t xml:space="preserve"> REGULATED_SC-Samples_certificates_DS</t>
   </si>
+  <si>
+    <t>If applicable, is the economic operator registered on an official list of approved economic operators or does it have an equivalent certificate (e.g. under a national (pre)qualification system)?</t>
+  </si>
+  <si>
+    <t>9b19e869-6c89-4cc4-bd6c-ac9ca8602165</t>
+  </si>
+  <si>
+    <t>CRITERION.OTHER.EO_DATA.REGISTERED_IN_OFFICIAL_LIST</t>
+  </si>
+  <si>
+    <t>64162276-7014-408f-a9af-080426bfe1fd</t>
+  </si>
+  <si>
+    <t>Please state the references on which the registration or certification is based, and, where applicable, the classification obtained in the official list</t>
+  </si>
+  <si>
+    <t>Does the registration or certification cover all the required selection criteria?</t>
+  </si>
 </sst>
 </file>
 
@@ -1819,7 +1838,7 @@
     <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="125">
+  <cellXfs count="135">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2149,6 +2168,36 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -35708,7 +35757,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -37178,7 +37227,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z53"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -39798,6 +39849,961 @@
   </hyperlinks>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Y135"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3" style="60" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" style="60" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" style="60" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" style="60" customWidth="1"/>
+    <col min="5" max="5" width="10" style="60" customWidth="1"/>
+    <col min="6" max="6" width="1.85546875" style="60" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="1.85546875" style="60" customWidth="1"/>
+    <col min="10" max="11" width="2.7109375" style="60" customWidth="1"/>
+    <col min="12" max="16" width="2.7109375" style="60" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.7109375" style="60" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" style="60" customWidth="1"/>
+    <col min="19" max="23" width="11.42578125" style="60"/>
+    <col min="24" max="24" width="11.42578125" style="125"/>
+    <col min="25" max="16384" width="11.42578125" style="60"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" s="125" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="16">
+        <v>1</v>
+      </c>
+      <c r="B1" s="17">
+        <v>2</v>
+      </c>
+      <c r="C1" s="16">
+        <v>3</v>
+      </c>
+      <c r="D1" s="17">
+        <v>4</v>
+      </c>
+      <c r="E1" s="16">
+        <v>5</v>
+      </c>
+      <c r="F1" s="17">
+        <v>6</v>
+      </c>
+      <c r="G1" s="16">
+        <v>7</v>
+      </c>
+      <c r="H1" s="17">
+        <v>8</v>
+      </c>
+      <c r="I1" s="16">
+        <v>9</v>
+      </c>
+      <c r="J1" s="17">
+        <v>10</v>
+      </c>
+      <c r="K1" s="16">
+        <v>11</v>
+      </c>
+      <c r="L1" s="17">
+        <v>12</v>
+      </c>
+      <c r="M1" s="16">
+        <v>13</v>
+      </c>
+      <c r="N1" s="17">
+        <v>14</v>
+      </c>
+      <c r="O1" s="16">
+        <v>15</v>
+      </c>
+      <c r="P1" s="17">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="16">
+        <v>17</v>
+      </c>
+      <c r="R1" s="17">
+        <v>18</v>
+      </c>
+      <c r="S1" s="16">
+        <v>19</v>
+      </c>
+      <c r="T1" s="17">
+        <v>20</v>
+      </c>
+      <c r="U1" s="16">
+        <v>21</v>
+      </c>
+      <c r="V1" s="17">
+        <v>22</v>
+      </c>
+      <c r="W1" s="16">
+        <v>23</v>
+      </c>
+      <c r="X1" s="92">
+        <v>24</v>
+      </c>
+      <c r="Y1" s="16">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" s="125" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="V2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="W2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="X2" s="72" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" s="125" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="49">
+        <v>57</v>
+      </c>
+      <c r="B3" s="51" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="51"/>
+      <c r="L3" s="51"/>
+      <c r="M3" s="51"/>
+      <c r="N3" s="51"/>
+      <c r="O3" s="51"/>
+      <c r="P3" s="51"/>
+      <c r="Q3" s="51"/>
+      <c r="R3" s="51"/>
+      <c r="S3" s="124" t="s">
+        <v>385</v>
+      </c>
+      <c r="T3" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="U3" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="V3" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="W3" s="124" t="s">
+        <v>386</v>
+      </c>
+      <c r="X3" s="124" t="s">
+        <v>387</v>
+      </c>
+      <c r="Y3" s="51" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" s="125" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="48" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="48" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="48"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="54"/>
+      <c r="L4" s="54"/>
+      <c r="M4" s="54"/>
+      <c r="N4" s="54"/>
+      <c r="O4" s="54"/>
+      <c r="P4" s="54"/>
+      <c r="Q4" s="54"/>
+      <c r="R4" s="126"/>
+      <c r="S4" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="T4" s="48" t="s">
+        <v>0</v>
+      </c>
+      <c r="U4" s="127">
+        <v>1</v>
+      </c>
+      <c r="V4" s="48" t="s">
+        <v>0</v>
+      </c>
+      <c r="W4" s="60" t="s">
+        <v>388</v>
+      </c>
+      <c r="X4" s="127" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y4" s="48" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" s="125" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="48" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="54" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="48" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="48"/>
+      <c r="K5" s="54"/>
+      <c r="L5" s="54"/>
+      <c r="M5" s="54"/>
+      <c r="N5" s="54"/>
+      <c r="O5" s="54"/>
+      <c r="P5" s="54"/>
+      <c r="Q5" s="54"/>
+      <c r="R5" s="126"/>
+      <c r="S5" s="48" t="s">
+        <v>181</v>
+      </c>
+      <c r="T5" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="U5" s="127">
+        <v>1</v>
+      </c>
+      <c r="V5" s="128" t="s">
+        <v>18</v>
+      </c>
+      <c r="W5" s="128" t="s">
+        <v>0</v>
+      </c>
+      <c r="X5" s="129" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="48" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" s="132" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="128" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="128" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="130"/>
+      <c r="D6" s="128" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="128"/>
+      <c r="F6" s="128"/>
+      <c r="G6" s="128"/>
+      <c r="H6" s="128"/>
+      <c r="I6" s="128"/>
+      <c r="J6" s="128"/>
+      <c r="K6" s="55"/>
+      <c r="L6" s="55"/>
+      <c r="M6" s="55"/>
+      <c r="N6" s="55"/>
+      <c r="O6" s="55"/>
+      <c r="P6" s="55"/>
+      <c r="Q6" s="55"/>
+      <c r="R6" s="130"/>
+      <c r="S6" s="48"/>
+      <c r="T6" s="48" t="s">
+        <v>0</v>
+      </c>
+      <c r="U6" s="127">
+        <v>1</v>
+      </c>
+      <c r="V6" s="128" t="s">
+        <v>0</v>
+      </c>
+      <c r="W6" s="131" t="s">
+        <v>47</v>
+      </c>
+      <c r="X6" s="129" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y6" s="128" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" s="132" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="128" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="128" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="130"/>
+      <c r="D7" s="128" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="128" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="128"/>
+      <c r="G7" s="128"/>
+      <c r="H7" s="128"/>
+      <c r="I7" s="128"/>
+      <c r="J7" s="128"/>
+      <c r="K7" s="55"/>
+      <c r="L7" s="55"/>
+      <c r="M7" s="55"/>
+      <c r="N7" s="55"/>
+      <c r="O7" s="55"/>
+      <c r="P7" s="55"/>
+      <c r="Q7" s="55"/>
+      <c r="R7" s="130"/>
+      <c r="S7" s="48" t="s">
+        <v>389</v>
+      </c>
+      <c r="T7" s="133" t="s">
+        <v>24</v>
+      </c>
+      <c r="U7" s="127">
+        <v>1</v>
+      </c>
+      <c r="V7" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="W7" s="128" t="s">
+        <v>0</v>
+      </c>
+      <c r="X7" s="127" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="128"/>
+    </row>
+    <row r="8" spans="1:25" s="132" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="128" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="128" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="130"/>
+      <c r="D8" s="128" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="128" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="128"/>
+      <c r="G8" s="128"/>
+      <c r="H8" s="128"/>
+      <c r="I8" s="128"/>
+      <c r="J8" s="128"/>
+      <c r="K8" s="55"/>
+      <c r="L8" s="55"/>
+      <c r="M8" s="55"/>
+      <c r="N8" s="55"/>
+      <c r="O8" s="55"/>
+      <c r="P8" s="55"/>
+      <c r="Q8" s="55"/>
+      <c r="R8" s="130"/>
+      <c r="S8" s="48" t="s">
+        <v>390</v>
+      </c>
+      <c r="T8" s="48"/>
+      <c r="U8" s="127">
+        <v>1</v>
+      </c>
+      <c r="V8" s="128" t="s">
+        <v>18</v>
+      </c>
+      <c r="W8" s="48"/>
+      <c r="X8" s="127" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="128" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" s="132" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="128" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="128" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="130"/>
+      <c r="D9" s="128" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" s="128"/>
+      <c r="F9" s="128"/>
+      <c r="G9" s="128"/>
+      <c r="H9" s="128"/>
+      <c r="I9" s="128"/>
+      <c r="J9" s="128"/>
+      <c r="K9" s="55"/>
+      <c r="L9" s="55"/>
+      <c r="M9" s="55"/>
+      <c r="N9" s="55"/>
+      <c r="O9" s="55"/>
+      <c r="P9" s="55"/>
+      <c r="Q9" s="55"/>
+      <c r="R9" s="130"/>
+      <c r="S9" s="48" t="s">
+        <v>0</v>
+      </c>
+      <c r="T9" s="48" t="s">
+        <v>0</v>
+      </c>
+      <c r="U9" s="127" t="s">
+        <v>0</v>
+      </c>
+      <c r="V9" s="48" t="s">
+        <v>0</v>
+      </c>
+      <c r="W9" s="48"/>
+      <c r="X9" s="127" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="128" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" s="132" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="128"/>
+      <c r="B10" s="128"/>
+      <c r="C10" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="128"/>
+      <c r="E10" s="128"/>
+      <c r="F10" s="128"/>
+      <c r="G10" s="128"/>
+      <c r="H10" s="128"/>
+      <c r="I10" s="128"/>
+      <c r="J10" s="128"/>
+      <c r="K10" s="55"/>
+      <c r="L10" s="55"/>
+      <c r="M10" s="55"/>
+      <c r="N10" s="55"/>
+      <c r="O10" s="55"/>
+      <c r="P10" s="55"/>
+      <c r="Q10" s="55"/>
+      <c r="R10" s="130"/>
+      <c r="S10" s="48"/>
+      <c r="T10" s="48"/>
+      <c r="U10" s="127"/>
+      <c r="V10" s="48"/>
+      <c r="W10" s="48"/>
+      <c r="X10" s="127"/>
+      <c r="Y10" s="128"/>
+    </row>
+    <row r="11" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="51" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="51"/>
+      <c r="D11" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="F11" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="G11" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="H11" s="51"/>
+      <c r="I11" s="51"/>
+      <c r="J11" s="51"/>
+      <c r="K11" s="51"/>
+      <c r="L11" s="51"/>
+      <c r="M11" s="51"/>
+      <c r="N11" s="51"/>
+      <c r="O11" s="51"/>
+      <c r="P11" s="51"/>
+      <c r="Q11" s="51"/>
+      <c r="R11" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="S11" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="T11" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="U11" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="V11" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="W11" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="X11" s="134" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="51" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X12" s="60"/>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X13" s="60"/>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X14" s="60"/>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X15" s="60"/>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X16" s="60"/>
+    </row>
+    <row r="17" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X17" s="60"/>
+    </row>
+    <row r="18" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X18" s="60"/>
+    </row>
+    <row r="19" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X19" s="60"/>
+    </row>
+    <row r="20" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X20" s="60"/>
+    </row>
+    <row r="21" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X21" s="60"/>
+    </row>
+    <row r="22" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X22" s="60"/>
+    </row>
+    <row r="23" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X23" s="60"/>
+    </row>
+    <row r="24" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X24" s="60"/>
+    </row>
+    <row r="25" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X25" s="60"/>
+    </row>
+    <row r="26" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X26" s="60"/>
+    </row>
+    <row r="27" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X27" s="60"/>
+    </row>
+    <row r="28" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X28" s="60"/>
+    </row>
+    <row r="29" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X29" s="60"/>
+    </row>
+    <row r="30" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X30" s="60"/>
+    </row>
+    <row r="31" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X31" s="60"/>
+    </row>
+    <row r="32" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X32" s="60"/>
+    </row>
+    <row r="33" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X33" s="60"/>
+    </row>
+    <row r="34" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X34" s="60"/>
+    </row>
+    <row r="35" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X35" s="60"/>
+    </row>
+    <row r="36" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X36" s="60"/>
+    </row>
+    <row r="37" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X37" s="60"/>
+    </row>
+    <row r="38" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X38" s="60"/>
+    </row>
+    <row r="39" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X39" s="60"/>
+    </row>
+    <row r="40" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X40" s="60"/>
+    </row>
+    <row r="41" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X41" s="60"/>
+    </row>
+    <row r="42" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X42" s="60"/>
+    </row>
+    <row r="43" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X43" s="60"/>
+    </row>
+    <row r="44" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X44" s="60"/>
+    </row>
+    <row r="45" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X45" s="60"/>
+    </row>
+    <row r="46" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X46" s="60"/>
+    </row>
+    <row r="47" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X47" s="60"/>
+    </row>
+    <row r="48" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X48" s="60"/>
+    </row>
+    <row r="49" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X49" s="60"/>
+    </row>
+    <row r="50" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X50" s="60"/>
+    </row>
+    <row r="51" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X51" s="60"/>
+    </row>
+    <row r="52" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X52" s="60"/>
+    </row>
+    <row r="53" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X53" s="60"/>
+    </row>
+    <row r="54" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X54" s="60"/>
+    </row>
+    <row r="55" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X55" s="60"/>
+    </row>
+    <row r="56" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X56" s="60"/>
+    </row>
+    <row r="57" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X57" s="60"/>
+    </row>
+    <row r="58" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X58" s="60"/>
+    </row>
+    <row r="59" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X59" s="60"/>
+    </row>
+    <row r="60" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X60" s="60"/>
+    </row>
+    <row r="61" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X61" s="60"/>
+    </row>
+    <row r="62" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X62" s="60"/>
+    </row>
+    <row r="63" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X63" s="60"/>
+    </row>
+    <row r="64" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X64" s="60"/>
+    </row>
+    <row r="65" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X65" s="60"/>
+    </row>
+    <row r="66" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X66" s="60"/>
+    </row>
+    <row r="67" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X67" s="60"/>
+    </row>
+    <row r="68" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X68" s="60"/>
+    </row>
+    <row r="69" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X69" s="60"/>
+    </row>
+    <row r="70" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X70" s="60"/>
+    </row>
+    <row r="71" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X71" s="60"/>
+    </row>
+    <row r="72" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X72" s="60"/>
+    </row>
+    <row r="73" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X73" s="60"/>
+    </row>
+    <row r="74" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X74" s="60"/>
+    </row>
+    <row r="75" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X75" s="60"/>
+    </row>
+    <row r="76" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X76" s="60"/>
+    </row>
+    <row r="77" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X77" s="60"/>
+    </row>
+    <row r="78" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X78" s="60"/>
+    </row>
+    <row r="79" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X79" s="60"/>
+    </row>
+    <row r="80" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X80" s="60"/>
+    </row>
+    <row r="81" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X81" s="60"/>
+    </row>
+    <row r="82" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X82" s="60"/>
+    </row>
+    <row r="83" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X83" s="60"/>
+    </row>
+    <row r="84" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X84" s="60"/>
+    </row>
+    <row r="85" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X85" s="60"/>
+    </row>
+    <row r="86" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X86" s="60"/>
+    </row>
+    <row r="87" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X87" s="60"/>
+    </row>
+    <row r="88" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X88" s="60"/>
+    </row>
+    <row r="89" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X89" s="60"/>
+    </row>
+    <row r="90" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X90" s="60"/>
+    </row>
+    <row r="91" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X91" s="60"/>
+    </row>
+    <row r="92" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X92" s="60"/>
+    </row>
+    <row r="93" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X93" s="60"/>
+    </row>
+    <row r="94" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X94" s="60"/>
+    </row>
+    <row r="95" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X95" s="60"/>
+    </row>
+    <row r="96" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X96" s="60"/>
+    </row>
+    <row r="97" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X97" s="60"/>
+    </row>
+    <row r="98" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X98" s="60"/>
+    </row>
+    <row r="99" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X99" s="60"/>
+    </row>
+    <row r="100" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X100" s="60"/>
+    </row>
+    <row r="101" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X101" s="60"/>
+    </row>
+    <row r="102" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X102" s="60"/>
+    </row>
+    <row r="103" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X103" s="60"/>
+    </row>
+    <row r="104" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X104" s="60"/>
+    </row>
+    <row r="105" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X105" s="60"/>
+    </row>
+    <row r="106" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X106" s="60"/>
+    </row>
+    <row r="107" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X107" s="60"/>
+    </row>
+    <row r="108" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X108" s="60"/>
+    </row>
+    <row r="109" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X109" s="60"/>
+    </row>
+    <row r="110" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X110" s="60"/>
+    </row>
+    <row r="111" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X111" s="60"/>
+    </row>
+    <row r="112" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X112" s="60"/>
+    </row>
+    <row r="113" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X113" s="60"/>
+    </row>
+    <row r="114" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X114" s="60"/>
+    </row>
+    <row r="115" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X115" s="60"/>
+    </row>
+    <row r="116" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X116" s="60"/>
+    </row>
+    <row r="117" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X117" s="60"/>
+    </row>
+    <row r="118" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X118" s="60"/>
+    </row>
+    <row r="119" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X119" s="60"/>
+    </row>
+    <row r="120" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X120" s="60"/>
+    </row>
+    <row r="121" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X121" s="60"/>
+    </row>
+    <row r="122" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X122" s="60"/>
+    </row>
+    <row r="123" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X123" s="60"/>
+    </row>
+    <row r="124" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X124" s="60"/>
+    </row>
+    <row r="125" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X125" s="60"/>
+    </row>
+    <row r="126" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X126" s="60"/>
+    </row>
+    <row r="127" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X127" s="60"/>
+    </row>
+    <row r="128" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X128" s="60"/>
+    </row>
+    <row r="129" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X129" s="60"/>
+    </row>
+    <row r="130" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X130" s="60"/>
+    </row>
+    <row r="131" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X131" s="60"/>
+    </row>
+    <row r="132" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X132" s="60"/>
+    </row>
+    <row r="133" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X133" s="60"/>
+    </row>
+    <row r="134" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X134" s="60"/>
+    </row>
+    <row r="135" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X135" s="60"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>